<commit_message>
Finalized changes to Front End SQL calls
</commit_message>
<xml_diff>
--- a/Project 2 Backend.xlsx
+++ b/Project 2 Backend.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="86">
   <si>
     <t>Id</t>
   </si>
@@ -147,112 +147,118 @@
     <t>cookie</t>
   </si>
   <si>
+    <t>dessert cup</t>
+  </si>
+  <si>
+    <t>dessert bowl</t>
+  </si>
+  <si>
+    <t>Made by Joshua</t>
+  </si>
+  <si>
+    <t>gatorade</t>
+  </si>
+  <si>
+    <t>By Joshua</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>calories</t>
+  </si>
+  <si>
+    <t>inventory</t>
+  </si>
+  <si>
+    <t>INSERT INTO entrees values(1007,'Chicken Fillet',5.49,310,100), (1008, 'Burger Fillet',4.49,310,100), (1009, 'Chicken Tender',1.60,300,100), (1010,'Black Bean Fillet',5.29,570,100), (1011,'Bun',2,200,100), (1012,'Letuce',0,0,100),(1013,'Tomato',0,0,100),(1014,'Pickles',0,0,100),(1015,'Onions',0,0,100),(1016,'American Cheese',0.5,100,100),(1017,'Swiss American Cheese',0.6,80,100),(1018,'Fries',2.69,240,100),(1019,'Bacon',0.9,90,100),(1020,'Meal Tray',0,0,100);</t>
+  </si>
+  <si>
+    <t>4.8 cost</t>
+  </si>
+  <si>
+    <t>6 for a burger</t>
+  </si>
+  <si>
+    <t>By Mohnish</t>
+  </si>
+  <si>
+    <t>id from entree</t>
+  </si>
+  <si>
+    <t>chocolate ice cream</t>
+  </si>
+  <si>
+    <t>vanilla ice cream</t>
+  </si>
+  <si>
+    <t>strawberry ice cream</t>
+  </si>
+  <si>
+    <t>cookie sandwich</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>PWD</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Pepsi</t>
+  </si>
+  <si>
+    <t>Diet pepsi</t>
+  </si>
+  <si>
+    <t>Gatorade</t>
+  </si>
+  <si>
+    <t>Mug Rootbeer</t>
+  </si>
+  <si>
+    <t>Sierra mist</t>
+  </si>
+  <si>
+    <t>Brisk</t>
+  </si>
+  <si>
+    <t>Drink Cup</t>
+  </si>
+  <si>
+    <t>Burger Fillet</t>
+  </si>
+  <si>
+    <t>Chicken Fillet</t>
+  </si>
+  <si>
+    <t>black bean fillet</t>
+  </si>
+  <si>
+    <t>-american-cheese</t>
+  </si>
+  <si>
+    <t>fries</t>
+  </si>
+  <si>
+    <t>cookies</t>
+  </si>
+  <si>
+    <t>dessert bowls</t>
+  </si>
+  <si>
     <t>dessert cups</t>
-  </si>
-  <si>
-    <t>dessert bowls</t>
-  </si>
-  <si>
-    <t>Made by Joshua</t>
-  </si>
-  <si>
-    <t>gatorade</t>
-  </si>
-  <si>
-    <t>By Joshua</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>price</t>
-  </si>
-  <si>
-    <t>calories</t>
-  </si>
-  <si>
-    <t>inventory</t>
-  </si>
-  <si>
-    <t>INSERT INTO entrees values(1007,'Chicken Fillet',5.49,310,100), (1008, 'Burger Fillet',4.49,310,100), (1009, 'Chicken Tender',1.60,300,100), (1010,'Black Bean Fillet',5.29,570,100), (1011,'Bun',2,200,100), (1012,'Letuce',0,0,100),(1013,'Tomato',0,0,100),(1014,'Pickles',0,0,100),(1015,'Onions',0,0,100),(1016,'American Cheese',0.5,100,100),(1017,'Swiss American Cheese',0.6,80,100),(1018,'Fries',2.69,240,100),(1019,'Bacon',0.9,90,100),(1020,'Meal Tray',0,0,100);</t>
-  </si>
-  <si>
-    <t>4.8 cost</t>
-  </si>
-  <si>
-    <t>6 for a burger</t>
-  </si>
-  <si>
-    <t>By Mohnish</t>
-  </si>
-  <si>
-    <t>id from entree</t>
-  </si>
-  <si>
-    <t>chocolate ice cream</t>
-  </si>
-  <si>
-    <t>vanilla ice cream</t>
-  </si>
-  <si>
-    <t>strawberry ice cream</t>
-  </si>
-  <si>
-    <t>cookie sandwich</t>
-  </si>
-  <si>
-    <t>dessert cup</t>
-  </si>
-  <si>
-    <t>dessert bowl</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Admin</t>
-  </si>
-  <si>
-    <t>PWD</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Pepsi</t>
-  </si>
-  <si>
-    <t>Diet pepsi</t>
-  </si>
-  <si>
-    <t>Gatorade</t>
-  </si>
-  <si>
-    <t>Mug Rootbeer</t>
-  </si>
-  <si>
-    <t>Sierra mist</t>
-  </si>
-  <si>
-    <t>Brisk</t>
-  </si>
-  <si>
-    <t>Drink Cup</t>
-  </si>
-  <si>
-    <t>black bean fillet</t>
-  </si>
-  <si>
-    <t>-american-cheese</t>
-  </si>
-  <si>
-    <t>fries</t>
-  </si>
-  <si>
-    <t>cookies</t>
   </si>
   <si>
     <t>Total Revenue</t>
@@ -362,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="35">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -425,15 +431,36 @@
     <xf borderId="0" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="8" fontId="1" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="8" fontId="4" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="8" fontId="1" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="8" fontId="1" numFmtId="165" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="7" fontId="1" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="8" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="8" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="8" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="8" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="8" fontId="1" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1302,29 +1329,37 @@
       </c>
     </row>
     <row r="38">
-      <c r="C38" s="1">
+      <c r="C38" s="8">
         <f t="shared" si="1"/>
         <v>1036</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
+      <c r="E38" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="F38" s="1">
+        <v>0.0</v>
+      </c>
       <c r="G38" s="2">
         <v>100.0</v>
       </c>
     </row>
     <row r="39">
-      <c r="C39" s="1">
+      <c r="C39" s="8">
         <f t="shared" si="1"/>
         <v>1037</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
+      <c r="E39" s="9">
+        <v>0.0</v>
+      </c>
+      <c r="F39" s="1">
+        <v>0.0</v>
+      </c>
       <c r="G39" s="3">
         <v>100.0</v>
       </c>
@@ -2319,13 +2354,13 @@
         <v>1036</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="E6" s="1">
         <v>0.0</v>
       </c>
       <c r="F6" s="1">
-        <v>475.0</v>
+        <v>0.0</v>
       </c>
       <c r="G6" s="2">
         <v>100.0</v>
@@ -2358,13 +2393,13 @@
         <v>1037</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="E7" s="9">
         <v>0.0</v>
       </c>
       <c r="F7" s="1">
-        <v>525.0</v>
+        <v>0.0</v>
       </c>
       <c r="G7" s="3">
         <v>100.0</v>
@@ -2417,7 +2452,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2.0" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B4" sqref="B4" pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
@@ -2449,43 +2487,43 @@
     </row>
     <row r="2">
       <c r="C2" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="F2" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="G2" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="H2" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="I2" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="J2" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="K2" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="L2" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="K2" s="15" t="s">
+      <c r="M2" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="L2" s="15" t="s">
+      <c r="N2" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="M2" s="15" t="s">
+      <c r="O2" s="16" t="s">
         <v>74</v>
-      </c>
-      <c r="N2" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="O2" s="16" t="s">
-        <v>13</v>
       </c>
       <c r="P2" s="16" t="s">
         <v>15</v>
@@ -2569,13 +2607,13 @@
         <v>78</v>
       </c>
       <c r="AQ2" s="18" t="s">
-        <v>44</v>
+        <v>79</v>
       </c>
       <c r="AR2" s="18" t="s">
-        <v>43</v>
+        <v>80</v>
       </c>
       <c r="AS2" s="19" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3">
@@ -2597,7 +2635,10 @@
       <c r="J3" s="20"/>
       <c r="K3" s="20"/>
       <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
+      <c r="M3" s="20">
+        <f>SUM(G3:L3)</f>
+        <v>5</v>
+      </c>
       <c r="N3" s="20"/>
       <c r="O3" s="20"/>
       <c r="P3" s="20"/>
@@ -2644,11 +2685,11 @@
       <c r="E4" s="20"/>
       <c r="F4" s="22"/>
       <c r="G4" s="24">
-        <f t="shared" ref="G4:AR4" si="1">G3*G1</f>
+        <f>$G3*G1</f>
         <v>7.25</v>
       </c>
       <c r="H4" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="H4:AR4" si="1">H3*H1</f>
         <v>0</v>
       </c>
       <c r="I4" s="24">
@@ -2669,7 +2710,7 @@
       </c>
       <c r="M4" s="25">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N4" s="20">
         <f t="shared" si="1"/>
@@ -2797,7 +2838,7 @@
       </c>
       <c r="AS4" s="26">
         <f>SUM(G4:AR4)</f>
-        <v>7.25</v>
+        <v>12.25</v>
       </c>
       <c r="AT4" s="21"/>
       <c r="AU4" s="20"/>
@@ -2813,21 +2854,318 @@
       <c r="F5" s="27">
         <v>44897.0</v>
       </c>
+      <c r="G5" s="21">
+        <v>5.0</v>
+      </c>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20">
+        <f>SUM(G5:L5)</f>
+        <v>5</v>
+      </c>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="20"/>
+      <c r="S5" s="20"/>
+      <c r="T5" s="20"/>
+      <c r="U5" s="20"/>
+      <c r="V5" s="20"/>
+      <c r="W5" s="20"/>
+      <c r="X5" s="20"/>
+      <c r="Y5" s="20"/>
+      <c r="Z5" s="20"/>
+      <c r="AA5" s="20"/>
+      <c r="AB5" s="20"/>
+      <c r="AC5" s="20"/>
+      <c r="AD5" s="20"/>
+      <c r="AE5" s="20"/>
+      <c r="AF5" s="20"/>
+      <c r="AG5" s="20"/>
+      <c r="AH5" s="20"/>
+      <c r="AI5" s="20"/>
+      <c r="AJ5" s="20"/>
+      <c r="AK5" s="20"/>
+      <c r="AL5" s="20"/>
+      <c r="AM5" s="20"/>
+      <c r="AN5" s="20"/>
+      <c r="AO5" s="20"/>
+      <c r="AP5" s="20"/>
+      <c r="AQ5" s="20"/>
+      <c r="AR5" s="20"/>
+      <c r="AS5" s="23"/>
     </row>
     <row r="6">
       <c r="F6" s="27"/>
+      <c r="G6" s="20">
+        <f>$G5*G3</f>
+        <v>25</v>
+      </c>
+      <c r="H6" s="20">
+        <f t="shared" ref="H6:AR6" si="2">H5*H3</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J6" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K6" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L6" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M6" s="20">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="N6" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O6" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P6" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R6" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S6" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T6" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U6" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="V6" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="W6" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="X6" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Y6" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Z6" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AA6" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AB6" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AC6" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AD6" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AE6" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AF6" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AG6" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AH6" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AI6" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AJ6" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AK6" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AL6" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AM6" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AN6" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AO6" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AP6" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AQ6" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AR6" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AS6" s="23">
+        <f>SUM(G6:AR6)</f>
+        <v>50</v>
+      </c>
     </row>
     <row r="7">
-      <c r="C7" s="8">
+      <c r="A7" s="20"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20">
         <f>C5+1</f>
         <v>2002</v>
       </c>
-      <c r="F7" s="27">
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="22">
         <v>44898.0</v>
       </c>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="20"/>
+      <c r="S7" s="20"/>
+      <c r="T7" s="20"/>
+      <c r="U7" s="20"/>
+      <c r="V7" s="20"/>
+      <c r="W7" s="20"/>
+      <c r="X7" s="20"/>
+      <c r="Y7" s="20"/>
+      <c r="Z7" s="20"/>
+      <c r="AA7" s="20"/>
+      <c r="AB7" s="20"/>
+      <c r="AC7" s="20"/>
+      <c r="AD7" s="20"/>
+      <c r="AE7" s="20"/>
+      <c r="AF7" s="20"/>
+      <c r="AG7" s="20"/>
+      <c r="AH7" s="20"/>
+      <c r="AI7" s="20"/>
+      <c r="AJ7" s="20"/>
+      <c r="AK7" s="20"/>
+      <c r="AL7" s="20"/>
+      <c r="AM7" s="20"/>
+      <c r="AN7" s="20"/>
+      <c r="AO7" s="20"/>
+      <c r="AP7" s="20"/>
+      <c r="AQ7" s="20"/>
+      <c r="AR7" s="20"/>
+      <c r="AS7" s="20"/>
+      <c r="AT7" s="20"/>
+      <c r="AU7" s="20"/>
+      <c r="AV7" s="20"/>
+      <c r="AW7" s="20"/>
+      <c r="AX7" s="20"/>
     </row>
     <row r="8">
-      <c r="F8" s="27"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="20"/>
+      <c r="R8" s="20"/>
+      <c r="S8" s="20"/>
+      <c r="T8" s="20"/>
+      <c r="U8" s="20"/>
+      <c r="V8" s="20"/>
+      <c r="W8" s="20"/>
+      <c r="X8" s="20"/>
+      <c r="Y8" s="20"/>
+      <c r="Z8" s="20"/>
+      <c r="AA8" s="20"/>
+      <c r="AB8" s="20"/>
+      <c r="AC8" s="20"/>
+      <c r="AD8" s="20"/>
+      <c r="AE8" s="20"/>
+      <c r="AF8" s="20"/>
+      <c r="AG8" s="20"/>
+      <c r="AH8" s="20"/>
+      <c r="AI8" s="20"/>
+      <c r="AJ8" s="20"/>
+      <c r="AK8" s="20"/>
+      <c r="AL8" s="20"/>
+      <c r="AM8" s="20"/>
+      <c r="AN8" s="20"/>
+      <c r="AO8" s="20"/>
+      <c r="AP8" s="20"/>
+      <c r="AQ8" s="20"/>
+      <c r="AR8" s="20"/>
+      <c r="AS8" s="20"/>
+      <c r="AT8" s="20"/>
+      <c r="AU8" s="20"/>
+      <c r="AV8" s="20"/>
+      <c r="AW8" s="20"/>
+      <c r="AX8" s="20"/>
     </row>
     <row r="9">
       <c r="C9" s="8">
@@ -2839,238 +3177,1141 @@
       </c>
     </row>
     <row r="10">
-      <c r="C10" s="8">
-        <f t="shared" ref="C10:C26" si="2">C9+1</f>
+      <c r="F10" s="27"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="20"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20">
+        <f>C9+1</f>
         <v>2004</v>
       </c>
-      <c r="F10" s="27">
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="22">
         <v>44900.0</v>
       </c>
-    </row>
-    <row r="11">
-      <c r="C11" s="8">
-        <f t="shared" si="2"/>
-        <v>2005</v>
-      </c>
-      <c r="F11" s="27">
-        <v>44901.0</v>
-      </c>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="20"/>
+      <c r="P11" s="20"/>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="20"/>
+      <c r="S11" s="20"/>
+      <c r="T11" s="20"/>
+      <c r="U11" s="20"/>
+      <c r="V11" s="20"/>
+      <c r="W11" s="20"/>
+      <c r="X11" s="20"/>
+      <c r="Y11" s="20"/>
+      <c r="Z11" s="20"/>
+      <c r="AA11" s="20"/>
+      <c r="AB11" s="20"/>
+      <c r="AC11" s="20"/>
+      <c r="AD11" s="20"/>
+      <c r="AE11" s="20"/>
+      <c r="AF11" s="20"/>
+      <c r="AG11" s="20"/>
+      <c r="AH11" s="20"/>
+      <c r="AI11" s="20"/>
+      <c r="AJ11" s="20"/>
+      <c r="AK11" s="20"/>
+      <c r="AL11" s="20"/>
+      <c r="AM11" s="20"/>
+      <c r="AN11" s="20"/>
+      <c r="AO11" s="20"/>
+      <c r="AP11" s="20"/>
+      <c r="AQ11" s="20"/>
+      <c r="AR11" s="20"/>
+      <c r="AS11" s="20"/>
+      <c r="AT11" s="20"/>
+      <c r="AU11" s="20"/>
+      <c r="AV11" s="20"/>
+      <c r="AW11" s="20"/>
+      <c r="AX11" s="20"/>
     </row>
     <row r="12">
-      <c r="B12" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C12" s="8">
-        <f t="shared" si="2"/>
-        <v>2006</v>
-      </c>
-      <c r="F12" s="27">
-        <v>44902.0</v>
-      </c>
+      <c r="A12" s="20"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="20"/>
+      <c r="Q12" s="20"/>
+      <c r="R12" s="20"/>
+      <c r="S12" s="20"/>
+      <c r="T12" s="20"/>
+      <c r="U12" s="20"/>
+      <c r="V12" s="20"/>
+      <c r="W12" s="20"/>
+      <c r="X12" s="20"/>
+      <c r="Y12" s="20"/>
+      <c r="Z12" s="20"/>
+      <c r="AA12" s="20"/>
+      <c r="AB12" s="20"/>
+      <c r="AC12" s="20"/>
+      <c r="AD12" s="20"/>
+      <c r="AE12" s="20"/>
+      <c r="AF12" s="20"/>
+      <c r="AG12" s="20"/>
+      <c r="AH12" s="20"/>
+      <c r="AI12" s="20"/>
+      <c r="AJ12" s="20"/>
+      <c r="AK12" s="20"/>
+      <c r="AL12" s="20"/>
+      <c r="AM12" s="20"/>
+      <c r="AN12" s="20"/>
+      <c r="AO12" s="20"/>
+      <c r="AP12" s="20"/>
+      <c r="AQ12" s="20"/>
+      <c r="AR12" s="20"/>
+      <c r="AS12" s="20"/>
+      <c r="AT12" s="20"/>
+      <c r="AU12" s="20"/>
+      <c r="AV12" s="20"/>
+      <c r="AW12" s="20"/>
+      <c r="AX12" s="20"/>
     </row>
     <row r="13">
       <c r="C13" s="8">
-        <f t="shared" si="2"/>
+        <f>C11+1</f>
+        <v>2005</v>
+      </c>
+      <c r="F13" s="27">
+        <v>44901.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="F14" s="27"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="20"/>
+      <c r="B15" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" s="20">
+        <f>C13+1</f>
+        <v>2006</v>
+      </c>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="22">
+        <v>44902.0</v>
+      </c>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="20"/>
+      <c r="N15" s="20"/>
+      <c r="O15" s="20"/>
+      <c r="P15" s="20"/>
+      <c r="Q15" s="20"/>
+      <c r="R15" s="20"/>
+      <c r="S15" s="20"/>
+      <c r="T15" s="20"/>
+      <c r="U15" s="20"/>
+      <c r="V15" s="20"/>
+      <c r="W15" s="20"/>
+      <c r="X15" s="20"/>
+      <c r="Y15" s="20"/>
+      <c r="Z15" s="20"/>
+      <c r="AA15" s="20"/>
+      <c r="AB15" s="20"/>
+      <c r="AC15" s="20"/>
+      <c r="AD15" s="20"/>
+      <c r="AE15" s="20"/>
+      <c r="AF15" s="20"/>
+      <c r="AG15" s="20"/>
+      <c r="AH15" s="20"/>
+      <c r="AI15" s="20"/>
+      <c r="AJ15" s="20"/>
+      <c r="AK15" s="20"/>
+      <c r="AL15" s="20"/>
+      <c r="AM15" s="20"/>
+      <c r="AN15" s="20"/>
+      <c r="AO15" s="20"/>
+      <c r="AP15" s="20"/>
+      <c r="AQ15" s="20"/>
+      <c r="AR15" s="20"/>
+      <c r="AS15" s="20"/>
+      <c r="AT15" s="20"/>
+      <c r="AU15" s="20"/>
+      <c r="AV15" s="20"/>
+      <c r="AW15" s="20"/>
+      <c r="AX15" s="20"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="20"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="20"/>
+      <c r="N16" s="20"/>
+      <c r="O16" s="20"/>
+      <c r="P16" s="20"/>
+      <c r="Q16" s="20"/>
+      <c r="R16" s="20"/>
+      <c r="S16" s="20"/>
+      <c r="T16" s="20"/>
+      <c r="U16" s="20"/>
+      <c r="V16" s="20"/>
+      <c r="W16" s="20"/>
+      <c r="X16" s="20"/>
+      <c r="Y16" s="20"/>
+      <c r="Z16" s="20"/>
+      <c r="AA16" s="20"/>
+      <c r="AB16" s="20"/>
+      <c r="AC16" s="20"/>
+      <c r="AD16" s="20"/>
+      <c r="AE16" s="20"/>
+      <c r="AF16" s="20"/>
+      <c r="AG16" s="20"/>
+      <c r="AH16" s="20"/>
+      <c r="AI16" s="20"/>
+      <c r="AJ16" s="20"/>
+      <c r="AK16" s="20"/>
+      <c r="AL16" s="20"/>
+      <c r="AM16" s="20"/>
+      <c r="AN16" s="20"/>
+      <c r="AO16" s="20"/>
+      <c r="AP16" s="20"/>
+      <c r="AQ16" s="20"/>
+      <c r="AR16" s="20"/>
+      <c r="AS16" s="20"/>
+      <c r="AT16" s="20"/>
+      <c r="AU16" s="20"/>
+      <c r="AV16" s="20"/>
+      <c r="AW16" s="20"/>
+      <c r="AX16" s="20"/>
+    </row>
+    <row r="17">
+      <c r="C17" s="8">
+        <f>C15+1</f>
         <v>2007</v>
       </c>
-      <c r="F13" s="27">
+      <c r="F17" s="27">
         <v>44903.0</v>
       </c>
     </row>
-    <row r="14">
-      <c r="C14" s="8">
-        <f t="shared" si="2"/>
+    <row r="18">
+      <c r="F18" s="27"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="20"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20">
+        <f>C17+1</f>
         <v>2008</v>
       </c>
-      <c r="F14" s="27">
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="22">
         <v>44904.0</v>
       </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="7"/>
-      <c r="C15" s="8">
-        <f t="shared" si="2"/>
-        <v>2009</v>
-      </c>
-      <c r="F15" s="27">
-        <v>44905.0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="7"/>
-      <c r="C16" s="8">
-        <f t="shared" si="2"/>
-        <v>2010</v>
-      </c>
-      <c r="F16" s="27">
-        <v>44906.0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="7"/>
-      <c r="C17" s="8">
-        <f t="shared" si="2"/>
-        <v>2011</v>
-      </c>
-      <c r="F17" s="27">
-        <v>44907.0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="7"/>
-      <c r="C18" s="8">
-        <f t="shared" si="2"/>
-        <v>2012</v>
-      </c>
-      <c r="F18" s="27">
-        <v>44908.0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="7"/>
-      <c r="C19" s="8">
-        <f t="shared" si="2"/>
-        <v>2013</v>
-      </c>
-      <c r="F19" s="27">
-        <v>44909.0</v>
-      </c>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="20"/>
+      <c r="N19" s="20"/>
+      <c r="O19" s="20"/>
+      <c r="P19" s="20"/>
+      <c r="Q19" s="20"/>
+      <c r="R19" s="20"/>
+      <c r="S19" s="20"/>
+      <c r="T19" s="20"/>
+      <c r="U19" s="20"/>
+      <c r="V19" s="20"/>
+      <c r="W19" s="20"/>
+      <c r="X19" s="20"/>
+      <c r="Y19" s="20"/>
+      <c r="Z19" s="20"/>
+      <c r="AA19" s="20"/>
+      <c r="AB19" s="20"/>
+      <c r="AC19" s="20"/>
+      <c r="AD19" s="20"/>
+      <c r="AE19" s="20"/>
+      <c r="AF19" s="20"/>
+      <c r="AG19" s="20"/>
+      <c r="AH19" s="20"/>
+      <c r="AI19" s="20"/>
+      <c r="AJ19" s="20"/>
+      <c r="AK19" s="20"/>
+      <c r="AL19" s="20"/>
+      <c r="AM19" s="20"/>
+      <c r="AN19" s="20"/>
+      <c r="AO19" s="20"/>
+      <c r="AP19" s="20"/>
+      <c r="AQ19" s="20"/>
+      <c r="AR19" s="20"/>
+      <c r="AS19" s="20"/>
+      <c r="AT19" s="20"/>
+      <c r="AU19" s="20"/>
+      <c r="AV19" s="20"/>
+      <c r="AW19" s="20"/>
+      <c r="AX19" s="20"/>
     </row>
     <row r="20">
-      <c r="A20" s="7"/>
-      <c r="C20" s="8">
-        <f t="shared" si="2"/>
-        <v>2014</v>
-      </c>
-      <c r="F20" s="27">
-        <v>44910.0</v>
-      </c>
+      <c r="A20" s="20"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="20"/>
+      <c r="N20" s="20"/>
+      <c r="O20" s="20"/>
+      <c r="P20" s="20"/>
+      <c r="Q20" s="20"/>
+      <c r="R20" s="20"/>
+      <c r="S20" s="20"/>
+      <c r="T20" s="20"/>
+      <c r="U20" s="20"/>
+      <c r="V20" s="20"/>
+      <c r="W20" s="20"/>
+      <c r="X20" s="20"/>
+      <c r="Y20" s="20"/>
+      <c r="Z20" s="20"/>
+      <c r="AA20" s="20"/>
+      <c r="AB20" s="20"/>
+      <c r="AC20" s="20"/>
+      <c r="AD20" s="20"/>
+      <c r="AE20" s="20"/>
+      <c r="AF20" s="20"/>
+      <c r="AG20" s="20"/>
+      <c r="AH20" s="20"/>
+      <c r="AI20" s="20"/>
+      <c r="AJ20" s="20"/>
+      <c r="AK20" s="20"/>
+      <c r="AL20" s="20"/>
+      <c r="AM20" s="20"/>
+      <c r="AN20" s="20"/>
+      <c r="AO20" s="20"/>
+      <c r="AP20" s="20"/>
+      <c r="AQ20" s="20"/>
+      <c r="AR20" s="20"/>
+      <c r="AS20" s="20"/>
+      <c r="AT20" s="20"/>
+      <c r="AU20" s="20"/>
+      <c r="AV20" s="20"/>
+      <c r="AW20" s="20"/>
+      <c r="AX20" s="20"/>
     </row>
     <row r="21">
       <c r="A21" s="7"/>
       <c r="C21" s="8">
-        <f t="shared" si="2"/>
-        <v>2015</v>
+        <f>C19+1</f>
+        <v>2009</v>
       </c>
       <c r="F21" s="27">
-        <v>44911.0</v>
+        <v>44905.0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="7"/>
-      <c r="C22" s="8">
-        <f t="shared" si="2"/>
+      <c r="F22" s="27"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="29"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20">
+        <f>C21+1</f>
+        <v>2010</v>
+      </c>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="22">
+        <v>44906.0</v>
+      </c>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
+      <c r="L23" s="20"/>
+      <c r="M23" s="20"/>
+      <c r="N23" s="20"/>
+      <c r="O23" s="20"/>
+      <c r="P23" s="20"/>
+      <c r="Q23" s="20"/>
+      <c r="R23" s="20"/>
+      <c r="S23" s="20"/>
+      <c r="T23" s="20"/>
+      <c r="U23" s="20"/>
+      <c r="V23" s="20"/>
+      <c r="W23" s="20"/>
+      <c r="X23" s="20"/>
+      <c r="Y23" s="20"/>
+      <c r="Z23" s="20"/>
+      <c r="AA23" s="20"/>
+      <c r="AB23" s="20"/>
+      <c r="AC23" s="20"/>
+      <c r="AD23" s="20"/>
+      <c r="AE23" s="20"/>
+      <c r="AF23" s="20"/>
+      <c r="AG23" s="20"/>
+      <c r="AH23" s="20"/>
+      <c r="AI23" s="20"/>
+      <c r="AJ23" s="20"/>
+      <c r="AK23" s="20"/>
+      <c r="AL23" s="20"/>
+      <c r="AM23" s="20"/>
+      <c r="AN23" s="20"/>
+      <c r="AO23" s="20"/>
+      <c r="AP23" s="20"/>
+      <c r="AQ23" s="20"/>
+      <c r="AR23" s="20"/>
+      <c r="AS23" s="20"/>
+      <c r="AT23" s="20"/>
+      <c r="AU23" s="20"/>
+      <c r="AV23" s="20"/>
+      <c r="AW23" s="20"/>
+      <c r="AX23" s="20"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="29"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
+      <c r="L24" s="20"/>
+      <c r="M24" s="20"/>
+      <c r="N24" s="20"/>
+      <c r="O24" s="20"/>
+      <c r="P24" s="20"/>
+      <c r="Q24" s="20"/>
+      <c r="R24" s="20"/>
+      <c r="S24" s="20"/>
+      <c r="T24" s="20"/>
+      <c r="U24" s="20"/>
+      <c r="V24" s="20"/>
+      <c r="W24" s="20"/>
+      <c r="X24" s="20"/>
+      <c r="Y24" s="20"/>
+      <c r="Z24" s="20"/>
+      <c r="AA24" s="20"/>
+      <c r="AB24" s="20"/>
+      <c r="AC24" s="20"/>
+      <c r="AD24" s="20"/>
+      <c r="AE24" s="20"/>
+      <c r="AF24" s="20"/>
+      <c r="AG24" s="20"/>
+      <c r="AH24" s="20"/>
+      <c r="AI24" s="20"/>
+      <c r="AJ24" s="20"/>
+      <c r="AK24" s="20"/>
+      <c r="AL24" s="20"/>
+      <c r="AM24" s="20"/>
+      <c r="AN24" s="20"/>
+      <c r="AO24" s="20"/>
+      <c r="AP24" s="20"/>
+      <c r="AQ24" s="20"/>
+      <c r="AR24" s="20"/>
+      <c r="AS24" s="20"/>
+      <c r="AT24" s="20"/>
+      <c r="AU24" s="20"/>
+      <c r="AV24" s="20"/>
+      <c r="AW24" s="20"/>
+      <c r="AX24" s="20"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="7"/>
+      <c r="C25" s="8">
+        <f>C23+1</f>
+        <v>2011</v>
+      </c>
+      <c r="F25" s="27">
+        <v>44907.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="7"/>
+      <c r="F26" s="27"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="29"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20">
+        <f>C25+1</f>
+        <v>2012</v>
+      </c>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="22">
+        <v>44908.0</v>
+      </c>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="20"/>
+      <c r="L27" s="20"/>
+      <c r="M27" s="20"/>
+      <c r="N27" s="20"/>
+      <c r="O27" s="20"/>
+      <c r="P27" s="20"/>
+      <c r="Q27" s="20"/>
+      <c r="R27" s="20"/>
+      <c r="S27" s="20"/>
+      <c r="T27" s="20"/>
+      <c r="U27" s="20"/>
+      <c r="V27" s="20"/>
+      <c r="W27" s="20"/>
+      <c r="X27" s="20"/>
+      <c r="Y27" s="20"/>
+      <c r="Z27" s="20"/>
+      <c r="AA27" s="20"/>
+      <c r="AB27" s="20"/>
+      <c r="AC27" s="20"/>
+      <c r="AD27" s="20"/>
+      <c r="AE27" s="20"/>
+      <c r="AF27" s="20"/>
+      <c r="AG27" s="20"/>
+      <c r="AH27" s="20"/>
+      <c r="AI27" s="20"/>
+      <c r="AJ27" s="20"/>
+      <c r="AK27" s="20"/>
+      <c r="AL27" s="20"/>
+      <c r="AM27" s="20"/>
+      <c r="AN27" s="20"/>
+      <c r="AO27" s="20"/>
+      <c r="AP27" s="20"/>
+      <c r="AQ27" s="20"/>
+      <c r="AR27" s="20"/>
+      <c r="AS27" s="20"/>
+      <c r="AT27" s="20"/>
+      <c r="AU27" s="20"/>
+      <c r="AV27" s="20"/>
+      <c r="AW27" s="20"/>
+      <c r="AX27" s="20"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="29"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="20"/>
+      <c r="L28" s="20"/>
+      <c r="M28" s="20"/>
+      <c r="N28" s="20"/>
+      <c r="O28" s="20"/>
+      <c r="P28" s="20"/>
+      <c r="Q28" s="20"/>
+      <c r="R28" s="20"/>
+      <c r="S28" s="20"/>
+      <c r="T28" s="20"/>
+      <c r="U28" s="20"/>
+      <c r="V28" s="20"/>
+      <c r="W28" s="20"/>
+      <c r="X28" s="20"/>
+      <c r="Y28" s="20"/>
+      <c r="Z28" s="20"/>
+      <c r="AA28" s="20"/>
+      <c r="AB28" s="20"/>
+      <c r="AC28" s="20"/>
+      <c r="AD28" s="20"/>
+      <c r="AE28" s="20"/>
+      <c r="AF28" s="20"/>
+      <c r="AG28" s="20"/>
+      <c r="AH28" s="20"/>
+      <c r="AI28" s="20"/>
+      <c r="AJ28" s="20"/>
+      <c r="AK28" s="20"/>
+      <c r="AL28" s="20"/>
+      <c r="AM28" s="20"/>
+      <c r="AN28" s="20"/>
+      <c r="AO28" s="20"/>
+      <c r="AP28" s="20"/>
+      <c r="AQ28" s="20"/>
+      <c r="AR28" s="20"/>
+      <c r="AS28" s="20"/>
+      <c r="AT28" s="20"/>
+      <c r="AU28" s="20"/>
+      <c r="AV28" s="20"/>
+      <c r="AW28" s="20"/>
+      <c r="AX28" s="20"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="7"/>
+      <c r="C29" s="8">
+        <f>C27+1</f>
+        <v>2013</v>
+      </c>
+      <c r="F29" s="27">
+        <v>44909.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="7"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="29"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20">
+        <f>C29+1</f>
+        <v>2014</v>
+      </c>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="22">
+        <v>44910.0</v>
+      </c>
+      <c r="G31" s="20"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="20"/>
+      <c r="K31" s="20"/>
+      <c r="L31" s="20"/>
+      <c r="M31" s="20"/>
+      <c r="N31" s="20"/>
+      <c r="O31" s="20"/>
+      <c r="P31" s="20"/>
+      <c r="Q31" s="20"/>
+      <c r="R31" s="20"/>
+      <c r="S31" s="20"/>
+      <c r="T31" s="20"/>
+      <c r="U31" s="20"/>
+      <c r="V31" s="20"/>
+      <c r="W31" s="20"/>
+      <c r="X31" s="20"/>
+      <c r="Y31" s="20"/>
+      <c r="Z31" s="20"/>
+      <c r="AA31" s="20"/>
+      <c r="AB31" s="20"/>
+      <c r="AC31" s="20"/>
+      <c r="AD31" s="20"/>
+      <c r="AE31" s="20"/>
+      <c r="AF31" s="20"/>
+      <c r="AG31" s="20"/>
+      <c r="AH31" s="20"/>
+      <c r="AI31" s="20"/>
+      <c r="AJ31" s="20"/>
+      <c r="AK31" s="20"/>
+      <c r="AL31" s="20"/>
+      <c r="AM31" s="20"/>
+      <c r="AN31" s="20"/>
+      <c r="AO31" s="20"/>
+      <c r="AP31" s="20"/>
+      <c r="AQ31" s="20"/>
+      <c r="AR31" s="20"/>
+      <c r="AS31" s="20"/>
+      <c r="AT31" s="20"/>
+      <c r="AU31" s="20"/>
+      <c r="AV31" s="20"/>
+      <c r="AW31" s="20"/>
+      <c r="AX31" s="20"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="29"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="20"/>
+      <c r="K32" s="20"/>
+      <c r="L32" s="20"/>
+      <c r="M32" s="20"/>
+      <c r="N32" s="20"/>
+      <c r="O32" s="20"/>
+      <c r="P32" s="20"/>
+      <c r="Q32" s="20"/>
+      <c r="R32" s="20"/>
+      <c r="S32" s="20"/>
+      <c r="T32" s="20"/>
+      <c r="U32" s="20"/>
+      <c r="V32" s="20"/>
+      <c r="W32" s="20"/>
+      <c r="X32" s="20"/>
+      <c r="Y32" s="20"/>
+      <c r="Z32" s="20"/>
+      <c r="AA32" s="20"/>
+      <c r="AB32" s="20"/>
+      <c r="AC32" s="20"/>
+      <c r="AD32" s="20"/>
+      <c r="AE32" s="20"/>
+      <c r="AF32" s="20"/>
+      <c r="AG32" s="20"/>
+      <c r="AH32" s="20"/>
+      <c r="AI32" s="20"/>
+      <c r="AJ32" s="20"/>
+      <c r="AK32" s="20"/>
+      <c r="AL32" s="20"/>
+      <c r="AM32" s="20"/>
+      <c r="AN32" s="20"/>
+      <c r="AO32" s="20"/>
+      <c r="AP32" s="20"/>
+      <c r="AQ32" s="20"/>
+      <c r="AR32" s="20"/>
+      <c r="AS32" s="20"/>
+      <c r="AT32" s="20"/>
+      <c r="AU32" s="20"/>
+      <c r="AV32" s="20"/>
+      <c r="AW32" s="20"/>
+      <c r="AX32" s="20"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="10"/>
+      <c r="C33" s="8">
+        <f>C31+1</f>
+        <v>2015</v>
+      </c>
+      <c r="F33" s="27">
+        <v>44911.0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="10"/>
+      <c r="F34" s="27"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="30"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="20">
+        <f>C33+1</f>
         <v>2016</v>
       </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="27">
+      <c r="D35" s="29"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="22">
         <v>44912.0</v>
       </c>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="7"/>
-      <c r="B23" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C23" s="8">
-        <f t="shared" si="2"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="20"/>
+      <c r="J35" s="20"/>
+      <c r="K35" s="20"/>
+      <c r="L35" s="20"/>
+      <c r="M35" s="20"/>
+      <c r="N35" s="20"/>
+      <c r="O35" s="20"/>
+      <c r="P35" s="20"/>
+      <c r="Q35" s="20"/>
+      <c r="R35" s="20"/>
+      <c r="S35" s="20"/>
+      <c r="T35" s="20"/>
+      <c r="U35" s="20"/>
+      <c r="V35" s="20"/>
+      <c r="W35" s="20"/>
+      <c r="X35" s="20"/>
+      <c r="Y35" s="20"/>
+      <c r="Z35" s="20"/>
+      <c r="AA35" s="20"/>
+      <c r="AB35" s="20"/>
+      <c r="AC35" s="20"/>
+      <c r="AD35" s="20"/>
+      <c r="AE35" s="20"/>
+      <c r="AF35" s="20"/>
+      <c r="AG35" s="20"/>
+      <c r="AH35" s="20"/>
+      <c r="AI35" s="20"/>
+      <c r="AJ35" s="20"/>
+      <c r="AK35" s="20"/>
+      <c r="AL35" s="20"/>
+      <c r="AM35" s="20"/>
+      <c r="AN35" s="20"/>
+      <c r="AO35" s="20"/>
+      <c r="AP35" s="20"/>
+      <c r="AQ35" s="20"/>
+      <c r="AR35" s="20"/>
+      <c r="AS35" s="20"/>
+      <c r="AT35" s="20"/>
+      <c r="AU35" s="20"/>
+      <c r="AV35" s="20"/>
+      <c r="AW35" s="20"/>
+      <c r="AX35" s="20"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="30"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="29"/>
+      <c r="E36" s="29"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="20"/>
+      <c r="I36" s="20"/>
+      <c r="J36" s="20"/>
+      <c r="K36" s="20"/>
+      <c r="L36" s="20"/>
+      <c r="M36" s="20"/>
+      <c r="N36" s="20"/>
+      <c r="O36" s="20"/>
+      <c r="P36" s="20"/>
+      <c r="Q36" s="20"/>
+      <c r="R36" s="20"/>
+      <c r="S36" s="20"/>
+      <c r="T36" s="20"/>
+      <c r="U36" s="20"/>
+      <c r="V36" s="20"/>
+      <c r="W36" s="20"/>
+      <c r="X36" s="20"/>
+      <c r="Y36" s="20"/>
+      <c r="Z36" s="20"/>
+      <c r="AA36" s="20"/>
+      <c r="AB36" s="20"/>
+      <c r="AC36" s="20"/>
+      <c r="AD36" s="20"/>
+      <c r="AE36" s="20"/>
+      <c r="AF36" s="20"/>
+      <c r="AG36" s="20"/>
+      <c r="AH36" s="20"/>
+      <c r="AI36" s="20"/>
+      <c r="AJ36" s="20"/>
+      <c r="AK36" s="20"/>
+      <c r="AL36" s="20"/>
+      <c r="AM36" s="20"/>
+      <c r="AN36" s="20"/>
+      <c r="AO36" s="20"/>
+      <c r="AP36" s="20"/>
+      <c r="AQ36" s="20"/>
+      <c r="AR36" s="20"/>
+      <c r="AS36" s="20"/>
+      <c r="AT36" s="20"/>
+      <c r="AU36" s="20"/>
+      <c r="AV36" s="20"/>
+      <c r="AW36" s="20"/>
+      <c r="AX36" s="20"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="10"/>
+      <c r="B37" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="C37" s="8">
+        <f>C35+1</f>
         <v>2017</v>
       </c>
-      <c r="F23" s="27">
+      <c r="F37" s="27">
         <v>44913.0</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="10"/>
-      <c r="C24" s="8">
-        <f t="shared" si="2"/>
+    <row r="38">
+      <c r="A38" s="10"/>
+      <c r="B38" s="31"/>
+      <c r="F38" s="27"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="29"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="20">
+        <f>C37+1</f>
         <v>2018</v>
       </c>
-      <c r="F24" s="27">
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="22">
         <v>44914.0</v>
       </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="10"/>
-      <c r="C25" s="8">
-        <f t="shared" si="2"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="20"/>
+      <c r="J39" s="20"/>
+      <c r="K39" s="20"/>
+      <c r="L39" s="20"/>
+      <c r="M39" s="20"/>
+      <c r="N39" s="20"/>
+      <c r="O39" s="20"/>
+      <c r="P39" s="20"/>
+      <c r="Q39" s="20"/>
+      <c r="R39" s="20"/>
+      <c r="S39" s="20"/>
+      <c r="T39" s="20"/>
+      <c r="U39" s="20"/>
+      <c r="V39" s="20"/>
+      <c r="W39" s="20"/>
+      <c r="X39" s="20"/>
+      <c r="Y39" s="20"/>
+      <c r="Z39" s="20"/>
+      <c r="AA39" s="20"/>
+      <c r="AB39" s="20"/>
+      <c r="AC39" s="20"/>
+      <c r="AD39" s="20"/>
+      <c r="AE39" s="20"/>
+      <c r="AF39" s="20"/>
+      <c r="AG39" s="20"/>
+      <c r="AH39" s="20"/>
+      <c r="AI39" s="20"/>
+      <c r="AJ39" s="20"/>
+      <c r="AK39" s="20"/>
+      <c r="AL39" s="20"/>
+      <c r="AM39" s="20"/>
+      <c r="AN39" s="20"/>
+      <c r="AO39" s="20"/>
+      <c r="AP39" s="20"/>
+      <c r="AQ39" s="20"/>
+      <c r="AR39" s="20"/>
+      <c r="AS39" s="20"/>
+      <c r="AT39" s="20"/>
+      <c r="AU39" s="20"/>
+      <c r="AV39" s="20"/>
+      <c r="AW39" s="20"/>
+      <c r="AX39" s="20"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="29"/>
+      <c r="B40" s="20"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="20"/>
+      <c r="J40" s="20"/>
+      <c r="K40" s="20"/>
+      <c r="L40" s="20"/>
+      <c r="M40" s="20"/>
+      <c r="N40" s="20"/>
+      <c r="O40" s="20"/>
+      <c r="P40" s="20"/>
+      <c r="Q40" s="20"/>
+      <c r="R40" s="20"/>
+      <c r="S40" s="20"/>
+      <c r="T40" s="20"/>
+      <c r="U40" s="20"/>
+      <c r="V40" s="20"/>
+      <c r="W40" s="20"/>
+      <c r="X40" s="20"/>
+      <c r="Y40" s="20"/>
+      <c r="Z40" s="20"/>
+      <c r="AA40" s="20"/>
+      <c r="AB40" s="20"/>
+      <c r="AC40" s="20"/>
+      <c r="AD40" s="20"/>
+      <c r="AE40" s="20"/>
+      <c r="AF40" s="20"/>
+      <c r="AG40" s="20"/>
+      <c r="AH40" s="20"/>
+      <c r="AI40" s="20"/>
+      <c r="AJ40" s="20"/>
+      <c r="AK40" s="20"/>
+      <c r="AL40" s="20"/>
+      <c r="AM40" s="20"/>
+      <c r="AN40" s="20"/>
+      <c r="AO40" s="20"/>
+      <c r="AP40" s="20"/>
+      <c r="AQ40" s="20"/>
+      <c r="AR40" s="20"/>
+      <c r="AS40" s="20"/>
+      <c r="AT40" s="20"/>
+      <c r="AU40" s="20"/>
+      <c r="AV40" s="20"/>
+      <c r="AW40" s="20"/>
+      <c r="AX40" s="20"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="7"/>
+      <c r="C41" s="8">
+        <f>C39+1</f>
         <v>2019</v>
       </c>
-      <c r="F25" s="27">
+      <c r="F41" s="27">
         <v>44915.0</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" s="10"/>
-      <c r="C26" s="8">
-        <f t="shared" si="2"/>
+    <row r="42">
+      <c r="A42" s="7"/>
+      <c r="F42" s="27"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="32"/>
+      <c r="B43" s="20"/>
+      <c r="C43" s="20">
+        <f>C41+1</f>
         <v>2020</v>
       </c>
-      <c r="F26" s="27">
+      <c r="D43" s="20"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="22">
         <v>44916.0</v>
       </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="7"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="H27" s="8">
-        <f>SUM(AS3:AS26)</f>
-        <v>7.25</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="7"/>
-      <c r="F28" s="27"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="3"/>
-      <c r="F29" s="27"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="3"/>
-      <c r="F30" s="27"/>
-    </row>
-    <row r="31">
-      <c r="A31" s="3"/>
-    </row>
-    <row r="32">
-      <c r="A32" s="3"/>
-    </row>
-    <row r="33">
-      <c r="A33" s="7"/>
-    </row>
-    <row r="34">
-      <c r="A34" s="7"/>
-    </row>
-    <row r="35">
-      <c r="A35" s="7"/>
-    </row>
-    <row r="36">
-      <c r="A36" s="7"/>
-    </row>
-    <row r="37">
-      <c r="A37" s="7"/>
+      <c r="G43" s="20"/>
+      <c r="H43" s="20"/>
+      <c r="I43" s="20"/>
+      <c r="J43" s="20"/>
+      <c r="K43" s="20"/>
+      <c r="L43" s="20"/>
+      <c r="M43" s="20"/>
+      <c r="N43" s="20"/>
+      <c r="O43" s="20"/>
+      <c r="P43" s="20"/>
+      <c r="Q43" s="20"/>
+      <c r="R43" s="20"/>
+      <c r="S43" s="20"/>
+      <c r="T43" s="20"/>
+      <c r="U43" s="20"/>
+      <c r="V43" s="20"/>
+      <c r="W43" s="20"/>
+      <c r="X43" s="20"/>
+      <c r="Y43" s="20"/>
+      <c r="Z43" s="20"/>
+      <c r="AA43" s="20"/>
+      <c r="AB43" s="20"/>
+      <c r="AC43" s="20"/>
+      <c r="AD43" s="20"/>
+      <c r="AE43" s="20"/>
+      <c r="AF43" s="20"/>
+      <c r="AG43" s="20"/>
+      <c r="AH43" s="20"/>
+      <c r="AI43" s="20"/>
+      <c r="AJ43" s="20"/>
+      <c r="AK43" s="20"/>
+      <c r="AL43" s="20"/>
+      <c r="AM43" s="20"/>
+      <c r="AN43" s="20"/>
+      <c r="AO43" s="20"/>
+      <c r="AP43" s="20"/>
+      <c r="AQ43" s="20"/>
+      <c r="AR43" s="20"/>
+      <c r="AS43" s="20"/>
+      <c r="AT43" s="20"/>
+      <c r="AU43" s="20"/>
+      <c r="AV43" s="20"/>
+      <c r="AW43" s="20"/>
+      <c r="AX43" s="20"/>
     </row>
     <row r="44">
-      <c r="A44" s="3"/>
+      <c r="A44" s="32"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="33"/>
+      <c r="G44" s="20"/>
+      <c r="H44" s="20"/>
+      <c r="I44" s="20"/>
+      <c r="J44" s="20"/>
+      <c r="K44" s="20"/>
+      <c r="L44" s="20"/>
+      <c r="M44" s="20"/>
+      <c r="N44" s="20"/>
+      <c r="O44" s="20"/>
+      <c r="P44" s="20"/>
+      <c r="Q44" s="20"/>
+      <c r="R44" s="20"/>
+      <c r="S44" s="20"/>
+      <c r="T44" s="20"/>
+      <c r="U44" s="20"/>
+      <c r="V44" s="20"/>
+      <c r="W44" s="20"/>
+      <c r="X44" s="20"/>
+      <c r="Y44" s="20"/>
+      <c r="Z44" s="20"/>
+      <c r="AA44" s="20"/>
+      <c r="AB44" s="20"/>
+      <c r="AC44" s="20"/>
+      <c r="AD44" s="20"/>
+      <c r="AE44" s="20"/>
+      <c r="AF44" s="20"/>
+      <c r="AG44" s="20"/>
+      <c r="AH44" s="20"/>
+      <c r="AI44" s="20"/>
+      <c r="AJ44" s="20"/>
+      <c r="AK44" s="20"/>
+      <c r="AL44" s="20"/>
+      <c r="AM44" s="20"/>
+      <c r="AN44" s="20"/>
+      <c r="AO44" s="20"/>
+      <c r="AP44" s="20"/>
+      <c r="AQ44" s="20"/>
+      <c r="AR44" s="20"/>
+      <c r="AS44" s="20"/>
+      <c r="AT44" s="20"/>
+      <c r="AU44" s="20"/>
+      <c r="AV44" s="20"/>
+      <c r="AW44" s="20"/>
+      <c r="AX44" s="20"/>
     </row>
     <row r="45">
       <c r="A45" s="3"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="3"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="7"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="7"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="7"/>
+      <c r="G49" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="H49" s="2">
+        <f>SUM(AS11:AS48)</f>
+        <v>0</v>
+      </c>
+      <c r="I49" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="J49" s="34" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="7"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="7"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="3"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="3"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>